<commit_message>
Updated ITA model - 2025-07-29 00:47
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD47E082-F4B0-4250-B3D6-D249F92DFBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB53522-D689-4D07-BDAB-15E568CCE188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -47,16 +48,40 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="87">
   <si>
     <t>bioenergy</t>
   </si>
@@ -251,6 +276,72 @@
   </si>
   <si>
     <t>-CO2Captured</t>
+  </si>
+  <si>
+    <t>Unnamed: 8</t>
+  </si>
+  <si>
+    <t>Unnamed: 9</t>
+  </si>
+  <si>
+    <t>Unnamed: 10</t>
+  </si>
+  <si>
+    <t>Unnamed: 11</t>
+  </si>
+  <si>
+    <t>Unnamed: 12</t>
+  </si>
+  <si>
+    <t>Unnamed: 13</t>
+  </si>
+  <si>
+    <t>Unnamed: 14</t>
+  </si>
+  <si>
+    <t>Unnamed: 15</t>
+  </si>
+  <si>
+    <t>Unnamed: 16</t>
+  </si>
+  <si>
+    <t>Unnamed: 17</t>
+  </si>
+  <si>
+    <t>Unnamed: 18</t>
+  </si>
+  <si>
+    <t>Unnamed: 19</t>
+  </si>
+  <si>
+    <t>Unnamed: 20</t>
+  </si>
+  <si>
+    <t>Unnamed: 21</t>
+  </si>
+  <si>
+    <t>Unnamed: 22</t>
+  </si>
+  <si>
+    <t>Unnamed: 23</t>
+  </si>
+  <si>
+    <t>Unnamed: 24</t>
+  </si>
+  <si>
+    <t>Unnamed: 25</t>
+  </si>
+  <si>
+    <t>Electricity Trade Data (TWh)</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>Import</t>
   </si>
 </sst>
 </file>
@@ -318,6 +409,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+  <rv s="1">
+    <v>13</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="propagated" t="b"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -718,14 +875,14 @@
       <c r="P4" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="4" cm="1">
+      <c r="Q4" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="Q4">MAX(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MAX(_xlpm.r))), historical_data!$C$24:$C$30=$P4))</f>
-        <v>0.62231700981598448</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="4" cm="1">
+      <c r="S4" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="S4">MIN(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MIN(_xlpm.r))), historical_data!$C$24:$C$30=$P4))</f>
-        <v>0.19733814732221869</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.45">
@@ -748,17 +905,17 @@
       <c r="P5" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="4" cm="1">
+      <c r="Q5" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="Q5">MAX(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MAX(_xlpm.r))), historical_data!$C$24:$C$30=$P5))</f>
-        <v>0.2955149688458561</v>
-      </c>
-      <c r="R5" s="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="4" t="e" vm="2">
         <f>IF(Q5&gt;0.7,Q5,0.7)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S5" s="4" cm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S5" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="S5">MIN(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MIN(_xlpm.r))), historical_data!$C$24:$C$30=$P5))</f>
-        <v>0.15844369919854487</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.45">
@@ -868,9 +1025,9 @@
       <c r="X8">
         <v>1</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="3" t="e" vm="2">
         <f>-Q4*$Q$1*8.76</f>
-        <v>-5.9966467065868265</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z8" s="3"/>
       <c r="AA8">
@@ -888,9 +1045,9 @@
       <c r="AF8">
         <v>1</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AG8" s="3" t="e" vm="2">
         <f>-S4*$S$1*8.76</f>
-        <v>-1.5558139534883721</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -912,13 +1069,13 @@
       <c r="X9">
         <v>1</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="3" t="e" vm="2">
         <f>-Q5*$Q$1*8.76</f>
-        <v>-2.8475822397986694</v>
-      </c>
-      <c r="Z9" s="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="3" t="e" vm="2">
         <f>-R5*$Q$1*8.76</f>
-        <v>-6.7451999999999996</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -935,9 +1092,9 @@
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="3" t="e" vm="2">
         <f>-S5*$S$1*8.76</f>
-        <v>-1.2491701244813276</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AI9">
         <v>0</v>
@@ -1109,7 +1266,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -1153,6 +1310,60 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -1337,1153 +1548,762 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>2000</v>
       </c>
       <c r="D13">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="E13">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F13">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="G13">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="H13">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="I13">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="J13">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="K13">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="L13">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="M13">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="N13">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="O13">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="P13">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="Q13">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="R13">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="S13">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="T13">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="U13">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="V13">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="W13">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="X13">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="Y13">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="Z13">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14">
         <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.29387335196920444</v>
-      </c>
-      <c r="E14">
-        <v>0.36119588962232163</v>
-      </c>
-      <c r="F14">
-        <v>0.44005793825548695</v>
-      </c>
-      <c r="G14">
-        <v>0.44668870313278031</v>
-      </c>
-      <c r="H14">
-        <v>0.54898593711379096</v>
-      </c>
-      <c r="I14">
-        <v>0.61000284572266994</v>
-      </c>
-      <c r="J14">
-        <v>0.64753472829655767</v>
-      </c>
-      <c r="K14">
-        <v>0.62752567747232946</v>
-      </c>
-      <c r="L14">
-        <v>0.58888908630393622</v>
-      </c>
-      <c r="M14">
-        <v>0.5673952378959225</v>
-      </c>
-      <c r="N14">
-        <v>0.59031104308580318</v>
-      </c>
-      <c r="O14">
-        <v>0.54674259382098878</v>
-      </c>
-      <c r="P14">
-        <v>0.44853889899451427</v>
-      </c>
-      <c r="Q14">
-        <v>0.58350948198641062</v>
-      </c>
-      <c r="R14">
-        <v>0.63667296066860524</v>
-      </c>
-      <c r="S14">
-        <v>0.65763867133730136</v>
-      </c>
-      <c r="T14">
-        <v>0.64758790186698112</v>
-      </c>
-      <c r="U14">
-        <v>0.64110341340216126</v>
-      </c>
-      <c r="V14">
-        <v>0.62627406907580729</v>
-      </c>
-      <c r="W14">
-        <v>0.64651878707642696</v>
-      </c>
-      <c r="X14">
-        <v>0.65169312541193969</v>
-      </c>
-      <c r="Y14">
-        <v>0.63648704525812538</v>
-      </c>
-      <c r="Z14">
-        <v>0.59277106311612904</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>0.91033975698475367</v>
-      </c>
-      <c r="E15">
-        <v>0.89790177468582399</v>
-      </c>
-      <c r="F15">
-        <v>0.79908675799086759</v>
-      </c>
-      <c r="G15">
-        <v>0.86238075862380759</v>
-      </c>
-      <c r="H15">
-        <v>0.96681069431997602</v>
-      </c>
-      <c r="I15">
-        <v>0.90583467733703538</v>
-      </c>
-      <c r="J15">
-        <v>0.94035447672321693</v>
-      </c>
-      <c r="K15">
-        <v>0.94745932262213428</v>
-      </c>
-      <c r="L15">
-        <v>0.93915491088745062</v>
-      </c>
-      <c r="M15">
-        <v>0.87740580138628832</v>
-      </c>
-      <c r="N15">
-        <v>0.84297945205479452</v>
-      </c>
-      <c r="O15">
-        <v>0.88662611646344525</v>
-      </c>
-      <c r="P15">
-        <v>0.87681346906518143</v>
-      </c>
-      <c r="Q15">
-        <v>0.88618737120343749</v>
-      </c>
-      <c r="R15">
-        <v>0.87940166595319624</v>
-      </c>
-      <c r="S15">
-        <v>0.91933192422945187</v>
-      </c>
-      <c r="T15">
-        <v>0.93594997410298097</v>
-      </c>
-      <c r="U15">
-        <v>0.922711274930198</v>
-      </c>
-      <c r="V15">
-        <v>0.90846117489425482</v>
-      </c>
-      <c r="W15">
-        <v>0.90391841519020266</v>
-      </c>
-      <c r="X15">
-        <v>0.89132060374858879</v>
-      </c>
-      <c r="Y15">
-        <v>0.87470664323539882</v>
-      </c>
-      <c r="Z15">
-        <v>0.86333726595725613</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16">
-        <v>0.28558245436146446</v>
-      </c>
-      <c r="E16">
-        <v>0.30125755131902554</v>
-      </c>
-      <c r="F16">
-        <v>0.26300120576970937</v>
-      </c>
-      <c r="G16">
-        <v>0.24464788133158288</v>
-      </c>
-      <c r="H16">
-        <v>0.27464620897146697</v>
-      </c>
-      <c r="I16">
-        <v>0.23342690659878584</v>
-      </c>
-      <c r="J16">
-        <v>0.23524997898052519</v>
-      </c>
-      <c r="K16">
-        <v>0.20802424867929775</v>
-      </c>
-      <c r="L16">
-        <v>0.25339148834066899</v>
-      </c>
-      <c r="M16">
-        <v>0.2854692026001181</v>
-      </c>
-      <c r="N16">
-        <v>0.28860623970905264</v>
-      </c>
-      <c r="O16">
-        <v>0.25080291521537151</v>
-      </c>
-      <c r="P16">
-        <v>0.22880093682435534</v>
-      </c>
-      <c r="Q16">
-        <v>0.28356807022282915</v>
-      </c>
-      <c r="R16">
-        <v>0.31127604163438005</v>
-      </c>
-      <c r="S16">
-        <v>0.24130564426305645</v>
-      </c>
-      <c r="T16">
-        <v>0.22657477726978403</v>
-      </c>
-      <c r="U16">
-        <v>0.19355715910404311</v>
-      </c>
-      <c r="V16">
-        <v>0.25624516880745851</v>
-      </c>
-      <c r="W16">
-        <v>0.24386476819833647</v>
-      </c>
-      <c r="X16">
-        <v>0.24895999115400089</v>
-      </c>
-      <c r="Y16">
-        <v>0.23824110380502575</v>
-      </c>
-      <c r="Z16">
-        <v>0.15125668935897063</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>0.18549363909037686</v>
-      </c>
-      <c r="E17">
-        <v>0.16242780220674277</v>
-      </c>
-      <c r="F17">
-        <v>0.18947752518915301</v>
-      </c>
-      <c r="G17">
-        <v>0.16134275900234468</v>
-      </c>
-      <c r="H17">
-        <v>0.12074365174832007</v>
-      </c>
-      <c r="I17">
-        <v>9.2604874927729272E-2</v>
-      </c>
-      <c r="J17">
-        <v>8.5383142670290207E-2</v>
-      </c>
-      <c r="K17">
-        <v>6.3942571567428885E-2</v>
-      </c>
-      <c r="L17">
-        <v>5.4351971653901113E-2</v>
-      </c>
-      <c r="M17">
-        <v>4.5120373132528896E-2</v>
-      </c>
-      <c r="N17">
-        <v>3.8445903076430775E-2</v>
-      </c>
-      <c r="O17">
-        <v>3.5465642257402952E-2</v>
-      </c>
-      <c r="P17">
-        <v>3.3828410664150516E-2</v>
-      </c>
-      <c r="Q17">
-        <v>2.9497986896519491E-2</v>
-      </c>
-      <c r="R17">
-        <v>2.8898030899281432E-2</v>
-      </c>
-      <c r="S17">
-        <v>2.9934943675673939E-2</v>
-      </c>
-      <c r="T17">
-        <v>2.9741012269575366E-2</v>
-      </c>
-      <c r="U17">
-        <v>2.8767224001894291E-2</v>
-      </c>
-      <c r="V17">
-        <v>2.7660265219492469E-2</v>
-      </c>
-      <c r="W17">
-        <v>2.5984909288337733E-2</v>
-      </c>
-      <c r="X17">
-        <v>2.5949170525979785E-2</v>
-      </c>
-      <c r="Y17">
-        <v>2.1681649145671975E-2</v>
-      </c>
-      <c r="Z17">
-        <v>3.1944135901513453E-2</v>
+        <v>86</v>
+      </c>
+      <c r="C15">
+        <v>44.35</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18">
-        <v>0.10814708002883922</v>
-      </c>
-      <c r="E18">
-        <v>0.10844748858447488</v>
-      </c>
-      <c r="F18">
-        <v>0.10896637608966378</v>
-      </c>
-      <c r="G18">
-        <v>0.10537407797681771</v>
-      </c>
-      <c r="H18">
-        <v>0.1067903962291943</v>
-      </c>
-      <c r="I18">
-        <v>0.10408272898200376</v>
-      </c>
-      <c r="J18">
-        <v>8.8787417554540851E-2</v>
-      </c>
-      <c r="K18">
-        <v>4.0424449979244499E-2</v>
-      </c>
-      <c r="L18">
-        <v>4.5606559081841996E-2</v>
-      </c>
-      <c r="M18">
-        <v>6.1094824721114389E-2</v>
-      </c>
-      <c r="N18">
-        <v>6.0783945108384398E-2</v>
-      </c>
-      <c r="O18">
-        <v>9.457878955568752E-2</v>
-      </c>
-      <c r="P18">
-        <v>0.12931650057322672</v>
-      </c>
-      <c r="Q18">
-        <v>0.13673327820166969</v>
-      </c>
-      <c r="R18">
-        <v>0.13816232692585365</v>
-      </c>
-      <c r="S18">
-        <v>0.13981618422725917</v>
-      </c>
-      <c r="T18">
-        <v>0.132076705674749</v>
-      </c>
-      <c r="U18">
-        <v>0.14275360852558924</v>
-      </c>
-      <c r="V18">
-        <v>0.12991755316197512</v>
-      </c>
-      <c r="W18">
-        <v>0.13118242254470275</v>
-      </c>
-      <c r="X18">
-        <v>0.13337047062172605</v>
-      </c>
-      <c r="Y18">
-        <v>0.12832090743979691</v>
-      </c>
-      <c r="Z18">
-        <v>0.13076711146608011</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>2000</v>
+      </c>
+      <c r="E19">
+        <v>2001</v>
+      </c>
+      <c r="F19">
+        <v>2002</v>
+      </c>
+      <c r="G19">
+        <v>2003</v>
+      </c>
+      <c r="H19">
+        <v>2004</v>
+      </c>
+      <c r="I19">
+        <v>2005</v>
+      </c>
+      <c r="J19">
+        <v>2006</v>
+      </c>
+      <c r="K19">
+        <v>2007</v>
+      </c>
+      <c r="L19">
+        <v>2008</v>
+      </c>
+      <c r="M19">
+        <v>2009</v>
+      </c>
+      <c r="N19">
+        <v>2010</v>
+      </c>
+      <c r="O19">
+        <v>2011</v>
+      </c>
+      <c r="P19">
+        <v>2012</v>
+      </c>
+      <c r="Q19">
+        <v>2013</v>
+      </c>
+      <c r="R19">
+        <v>2014</v>
+      </c>
+      <c r="S19">
+        <v>2015</v>
+      </c>
+      <c r="T19">
+        <v>2016</v>
+      </c>
+      <c r="U19">
+        <v>2017</v>
+      </c>
+      <c r="V19">
+        <v>2018</v>
+      </c>
+      <c r="W19">
+        <v>2019</v>
+      </c>
+      <c r="X19">
+        <v>2020</v>
+      </c>
+      <c r="Y19">
+        <v>2021</v>
+      </c>
+      <c r="Z19">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>0.17705070631596159</v>
-      </c>
-      <c r="E19">
-        <v>0.20269433899983494</v>
-      </c>
-      <c r="F19">
-        <v>0.20547945205479451</v>
-      </c>
-      <c r="G19">
-        <v>0.19043290178991254</v>
-      </c>
-      <c r="H19">
-        <v>0.1867689303237674</v>
-      </c>
-      <c r="I19">
-        <v>0.1634194908745619</v>
-      </c>
-      <c r="J19">
-        <v>0.1781260653289736</v>
-      </c>
-      <c r="K19">
-        <v>0.17044532377504912</v>
-      </c>
-      <c r="L19">
-        <v>0.15732740697561451</v>
-      </c>
-      <c r="M19">
-        <v>0.15299618343829349</v>
-      </c>
-      <c r="N19">
-        <v>0.17972438028317755</v>
-      </c>
-      <c r="O19">
-        <v>0.16251183135517033</v>
-      </c>
-      <c r="P19">
-        <v>0.18890322756994438</v>
-      </c>
-      <c r="Q19">
-        <v>0.19908293588810169</v>
-      </c>
-      <c r="R19">
-        <v>0.19954897961008153</v>
-      </c>
-      <c r="S19">
-        <v>0.18545551905719279</v>
-      </c>
-      <c r="T19">
-        <v>0.21518058037191448</v>
-      </c>
-      <c r="U19">
-        <v>0.20801272044711919</v>
-      </c>
-      <c r="V19">
-        <v>0.19769064914008325</v>
-      </c>
-      <c r="W19">
-        <v>0.21594436217582091</v>
-      </c>
-      <c r="X19">
-        <v>0.19702002802981769</v>
-      </c>
-      <c r="Y19">
-        <v>0.21228169618742199</v>
-      </c>
-      <c r="Z19">
-        <v>0.19792026167823587</v>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.29387335196920444</v>
+      </c>
+      <c r="E20">
+        <v>0.36119588962232163</v>
+      </c>
+      <c r="F20">
+        <v>0.44005793825548695</v>
+      </c>
+      <c r="G20">
+        <v>0.44668870313278031</v>
+      </c>
+      <c r="H20">
+        <v>0.54898593711379096</v>
+      </c>
+      <c r="I20">
+        <v>0.61000284572266994</v>
+      </c>
+      <c r="J20">
+        <v>0.64753472829655767</v>
+      </c>
+      <c r="K20">
+        <v>0.62752567747232946</v>
+      </c>
+      <c r="L20">
+        <v>0.58888908630393622</v>
+      </c>
+      <c r="M20">
+        <v>0.5673952378959225</v>
+      </c>
+      <c r="N20">
+        <v>0.59031104308580318</v>
+      </c>
+      <c r="O20">
+        <v>0.54674259382098878</v>
+      </c>
+      <c r="P20">
+        <v>0.44853889899451427</v>
+      </c>
+      <c r="Q20">
+        <v>0.58350948198641062</v>
+      </c>
+      <c r="R20">
+        <v>0.63667296066860524</v>
+      </c>
+      <c r="S20">
+        <v>0.65763867133730136</v>
+      </c>
+      <c r="T20">
+        <v>0.64758790186698112</v>
+      </c>
+      <c r="U20">
+        <v>0.64110341340216126</v>
+      </c>
+      <c r="V20">
+        <v>0.62627406907580729</v>
+      </c>
+      <c r="W20">
+        <v>0.64651878707642696</v>
+      </c>
+      <c r="X20">
+        <v>0.65169312541193969</v>
+      </c>
+      <c r="Y20">
+        <v>0.63648704525812538</v>
+      </c>
+      <c r="Z20">
+        <v>0.59277106311612904</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>0.91033975698475367</v>
+      </c>
+      <c r="E21">
+        <v>0.89790177468582399</v>
+      </c>
+      <c r="F21">
+        <v>0.79908675799086759</v>
+      </c>
+      <c r="G21">
+        <v>0.86238075862380759</v>
+      </c>
+      <c r="H21">
+        <v>0.96681069431997602</v>
+      </c>
+      <c r="I21">
+        <v>0.90583467733703538</v>
+      </c>
+      <c r="J21">
+        <v>0.94035447672321693</v>
+      </c>
+      <c r="K21">
+        <v>0.94745932262213428</v>
+      </c>
+      <c r="L21">
+        <v>0.93915491088745062</v>
+      </c>
+      <c r="M21">
+        <v>0.87740580138628832</v>
+      </c>
+      <c r="N21">
+        <v>0.84297945205479452</v>
+      </c>
+      <c r="O21">
+        <v>0.88662611646344525</v>
+      </c>
+      <c r="P21">
+        <v>0.87681346906518143</v>
+      </c>
+      <c r="Q21">
+        <v>0.88618737120343749</v>
+      </c>
+      <c r="R21">
+        <v>0.87940166595319624</v>
+      </c>
+      <c r="S21">
+        <v>0.91933192422945187</v>
+      </c>
+      <c r="T21">
+        <v>0.93594997410298097</v>
+      </c>
+      <c r="U21">
+        <v>0.922711274930198</v>
+      </c>
+      <c r="V21">
+        <v>0.90846117489425482</v>
+      </c>
+      <c r="W21">
+        <v>0.90391841519020266</v>
+      </c>
+      <c r="X21">
+        <v>0.89132060374858879</v>
+      </c>
+      <c r="Y21">
+        <v>0.87470664323539882</v>
+      </c>
+      <c r="Z21">
+        <v>0.86333726595725613</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>0.28558245436146446</v>
+      </c>
+      <c r="E22">
+        <v>0.30125755131902554</v>
+      </c>
+      <c r="F22">
+        <v>0.26300120576970937</v>
+      </c>
+      <c r="G22">
+        <v>0.24464788133158288</v>
+      </c>
+      <c r="H22">
+        <v>0.27464620897146697</v>
+      </c>
+      <c r="I22">
+        <v>0.23342690659878584</v>
+      </c>
+      <c r="J22">
+        <v>0.23524997898052519</v>
+      </c>
+      <c r="K22">
+        <v>0.20802424867929775</v>
+      </c>
+      <c r="L22">
+        <v>0.25339148834066899</v>
+      </c>
+      <c r="M22">
+        <v>0.2854692026001181</v>
+      </c>
+      <c r="N22">
+        <v>0.28860623970905264</v>
+      </c>
+      <c r="O22">
+        <v>0.25080291521537151</v>
+      </c>
+      <c r="P22">
+        <v>0.22880093682435534</v>
+      </c>
+      <c r="Q22">
+        <v>0.28356807022282915</v>
+      </c>
+      <c r="R22">
+        <v>0.31127604163438005</v>
+      </c>
+      <c r="S22">
+        <v>0.24130564426305645</v>
+      </c>
+      <c r="T22">
+        <v>0.22657477726978403</v>
+      </c>
+      <c r="U22">
+        <v>0.19355715910404311</v>
+      </c>
+      <c r="V22">
+        <v>0.25624516880745851</v>
+      </c>
+      <c r="W22">
+        <v>0.24386476819833647</v>
+      </c>
+      <c r="X22">
+        <v>0.24895999115400089</v>
+      </c>
+      <c r="Y22">
+        <v>0.23824110380502575</v>
+      </c>
+      <c r="Z22">
+        <v>0.15125668935897063</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>2000</v>
+        <v>0.18549363909037686</v>
       </c>
       <c r="E23">
-        <v>2001</v>
+        <v>0.16242780220674277</v>
       </c>
       <c r="F23">
-        <v>2002</v>
+        <v>0.18947752518915301</v>
       </c>
       <c r="G23">
-        <v>2003</v>
+        <v>0.16134275900234468</v>
       </c>
       <c r="H23">
-        <v>2004</v>
+        <v>0.12074365174832007</v>
       </c>
       <c r="I23">
-        <v>2005</v>
+        <v>9.2604874927729272E-2</v>
       </c>
       <c r="J23">
-        <v>2006</v>
+        <v>8.5383142670290207E-2</v>
       </c>
       <c r="K23">
-        <v>2007</v>
+        <v>6.3942571567428885E-2</v>
       </c>
       <c r="L23">
-        <v>2008</v>
+        <v>5.4351971653901113E-2</v>
       </c>
       <c r="M23">
-        <v>2009</v>
+        <v>4.5120373132528896E-2</v>
       </c>
       <c r="N23">
-        <v>2010</v>
+        <v>3.8445903076430775E-2</v>
       </c>
       <c r="O23">
-        <v>2011</v>
+        <v>3.5465642257402952E-2</v>
       </c>
       <c r="P23">
-        <v>2012</v>
+        <v>3.3828410664150516E-2</v>
       </c>
       <c r="Q23">
-        <v>2013</v>
+        <v>2.9497986896519491E-2</v>
       </c>
       <c r="R23">
-        <v>2014</v>
+        <v>2.8898030899281432E-2</v>
       </c>
       <c r="S23">
-        <v>2015</v>
+        <v>2.9934943675673939E-2</v>
       </c>
       <c r="T23">
-        <v>2016</v>
+        <v>2.9741012269575366E-2</v>
       </c>
       <c r="U23">
-        <v>2017</v>
+        <v>2.8767224001894291E-2</v>
       </c>
       <c r="V23">
-        <v>2018</v>
+        <v>2.7660265219492469E-2</v>
       </c>
       <c r="W23">
-        <v>2019</v>
+        <v>2.5984909288337733E-2</v>
       </c>
       <c r="X23">
-        <v>2020</v>
+        <v>2.5949170525979785E-2</v>
       </c>
       <c r="Y23">
-        <v>2021</v>
+        <v>2.1681649145671975E-2</v>
       </c>
       <c r="Z23">
-        <v>2022</v>
-      </c>
-      <c r="AA23">
-        <v>2023</v>
+        <v>3.1944135901513453E-2</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D24">
-        <v>0.61522608801066792</v>
+        <v>0.10814708002883922</v>
       </c>
       <c r="E24">
-        <v>0.62934286281516771</v>
+        <v>0.10844748858447488</v>
       </c>
       <c r="F24">
-        <v>0.61410525614105249</v>
+        <v>0.10896637608966378</v>
       </c>
       <c r="G24">
-        <v>0.63330715760695699</v>
+        <v>0.10537407797681771</v>
       </c>
       <c r="H24">
-        <v>0.72548666186012989</v>
+        <v>0.1067903962291943</v>
       </c>
       <c r="I24">
-        <v>0.74052659669098031</v>
+        <v>0.10408272898200376</v>
       </c>
       <c r="J24">
-        <v>0.77363813512491642</v>
+        <v>8.8787417554540851E-2</v>
       </c>
       <c r="K24">
-        <v>0.75846709807546864</v>
+        <v>4.0424449979244499E-2</v>
       </c>
       <c r="L24">
-        <v>0.71674526536417393</v>
+        <v>4.5606559081841996E-2</v>
       </c>
       <c r="M24">
-        <v>0.66333456744415642</v>
+        <v>6.1094824721114389E-2</v>
       </c>
       <c r="N24">
-        <v>0.66085188356164382</v>
+        <v>6.0783945108384398E-2</v>
       </c>
       <c r="O24">
-        <v>0.62919014676012885</v>
+        <v>9.457878955568752E-2</v>
       </c>
       <c r="P24">
-        <v>0.52921203606135103</v>
+        <v>0.12931650057322672</v>
       </c>
       <c r="Q24">
-        <v>0.63624764974482939</v>
+        <v>0.13673327820166969</v>
       </c>
       <c r="R24">
-        <v>0.68106183731909309</v>
+        <v>0.13816232692585365</v>
       </c>
       <c r="S24">
-        <v>0.70676749919842574</v>
+        <v>0.13981618422725917</v>
       </c>
       <c r="T24">
-        <v>0.69930259547283602</v>
+        <v>0.132076705674749</v>
       </c>
       <c r="U24">
-        <v>0.69169425869419376</v>
+        <v>0.14275360852558924</v>
       </c>
       <c r="V24">
-        <v>0.67662443458314581</v>
+        <v>0.12991755316197512</v>
       </c>
       <c r="W24">
-        <v>0.69304680906316962</v>
+        <v>0.13118242254470275</v>
       </c>
       <c r="X24">
-        <v>0.69550645885530227</v>
+        <v>0.13337047062172605</v>
       </c>
       <c r="Y24">
-        <v>0.68029990954762931</v>
+        <v>0.12832090743979691</v>
       </c>
       <c r="Z24">
-        <v>0.64195219167132056</v>
-      </c>
-      <c r="AA24">
-        <v>0.60575494311218137</v>
+        <v>0.13076711146608011</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>0.34602076124567482</v>
+        <v>0.17705070631596159</v>
       </c>
       <c r="E25">
-        <v>0.42117978124668154</v>
+        <v>0.20269433899983494</v>
       </c>
       <c r="F25">
-        <v>0.47055856429860893</v>
+        <v>0.20547945205479451</v>
       </c>
       <c r="G25">
-        <v>0.51515875544228529</v>
+        <v>0.19043290178991254</v>
       </c>
       <c r="H25">
-        <v>0.62231700981598448</v>
+        <v>0.1867689303237674</v>
       </c>
       <c r="I25">
-        <v>0.57221959796357535</v>
+        <v>0.1634194908745619</v>
       </c>
       <c r="J25">
-        <v>0.58009237390437207</v>
+        <v>0.1781260653289736</v>
       </c>
       <c r="K25">
-        <v>0.57878024458090593</v>
+        <v>0.17044532377504912</v>
       </c>
       <c r="L25">
-        <v>0.61000827129859381</v>
+        <v>0.15732740697561451</v>
       </c>
       <c r="M25">
-        <v>0.52024422939968995</v>
+        <v>0.15299618343829349</v>
       </c>
       <c r="N25">
-        <v>0.45490352335545442</v>
+        <v>0.17972438028317755</v>
       </c>
       <c r="O25">
-        <v>0.51215289704730615</v>
+        <v>0.16251183135517033</v>
       </c>
       <c r="P25">
-        <v>0.56264684464351955</v>
+        <v>0.18890322756994438</v>
       </c>
       <c r="Q25">
-        <v>0.51638935070050329</v>
+        <v>0.19908293588810169</v>
       </c>
       <c r="R25">
-        <v>0.50458246816891728</v>
+        <v>0.19954897961008153</v>
       </c>
       <c r="S25">
-        <v>0.50892743542983165</v>
+        <v>0.18545551905719279</v>
       </c>
       <c r="T25">
-        <v>0.46671280059135295</v>
+        <v>0.21518058037191448</v>
       </c>
       <c r="U25">
-        <v>0.43565916312852143</v>
+        <v>0.20801272044711919</v>
       </c>
       <c r="V25">
-        <v>0.38011695906432741</v>
+        <v>0.19769064914008325</v>
       </c>
       <c r="W25">
-        <v>0.25154209725226306</v>
+        <v>0.21594436217582091</v>
       </c>
       <c r="X25">
-        <v>0.19733814732221869</v>
+        <v>0.19702002802981769</v>
       </c>
       <c r="Y25">
-        <v>0.23501565653517861</v>
+        <v>0.21228169618742199</v>
       </c>
       <c r="Z25">
-        <v>0.37900884409845853</v>
-      </c>
-      <c r="AA25">
-        <v>0.25717309414385414</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>0.21688427845750258</v>
-      </c>
-      <c r="E26">
-        <v>0.22202418548512892</v>
-      </c>
-      <c r="F26">
-        <v>0.21195692035826924</v>
-      </c>
-      <c r="G26">
-        <v>0.2444397765407833</v>
-      </c>
-      <c r="H26">
-        <v>0.25723564401629956</v>
-      </c>
-      <c r="I26">
-        <v>0.28042118198664318</v>
-      </c>
-      <c r="J26">
-        <v>0.28071079794005777</v>
-      </c>
-      <c r="K26">
-        <v>0.2922584260992816</v>
-      </c>
-      <c r="L26">
-        <v>0.2779788969658355</v>
-      </c>
-      <c r="M26">
-        <v>0.23646215642703375</v>
-      </c>
-      <c r="N26">
-        <v>0.24074060070301742</v>
-      </c>
-      <c r="O26">
-        <v>0.22510363173419468</v>
-      </c>
-      <c r="P26">
-        <v>0.20133855684813015</v>
-      </c>
-      <c r="Q26">
-        <v>0.17523112617091591</v>
-      </c>
-      <c r="R26">
-        <v>0.15844369919854487</v>
-      </c>
-      <c r="S26">
-        <v>0.20478133387114289</v>
-      </c>
-      <c r="T26">
-        <v>0.24738866431689593</v>
-      </c>
-      <c r="U26">
-        <v>0.2791433980876013</v>
-      </c>
-      <c r="V26">
-        <v>0.25589885068453339</v>
-      </c>
-      <c r="W26">
-        <v>0.28175925948019492</v>
-      </c>
-      <c r="X26">
-        <v>0.27138259384113744</v>
-      </c>
-      <c r="Y26">
-        <v>0.2955149688458561</v>
-      </c>
-      <c r="Z26">
-        <v>0.2867461537463678</v>
-      </c>
-      <c r="AA26">
-        <v>0.23584379225019769</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27">
-        <v>0.30785003663554733</v>
-      </c>
-      <c r="E27">
-        <v>0.3246419991455694</v>
-      </c>
-      <c r="F27">
-        <v>0.27242847373877754</v>
-      </c>
-      <c r="G27">
-        <v>0.25066305744675033</v>
-      </c>
-      <c r="H27">
-        <v>0.2878697637482629</v>
-      </c>
-      <c r="I27">
-        <v>0.24164201341994127</v>
-      </c>
-      <c r="J27">
-        <v>0.24679151021192447</v>
-      </c>
-      <c r="K27">
-        <v>0.21833189641408821</v>
-      </c>
-      <c r="L27">
-        <v>0.27431533213114406</v>
-      </c>
-      <c r="M27">
-        <v>0.32220499948856351</v>
-      </c>
-      <c r="N27">
-        <v>0.33232439853964491</v>
-      </c>
-      <c r="O27">
-        <v>0.29418411739628436</v>
-      </c>
-      <c r="P27">
-        <v>0.26672323467058051</v>
-      </c>
-      <c r="Q27">
-        <v>0.33373809433461088</v>
-      </c>
-      <c r="R27">
-        <v>0.36886258026147345</v>
-      </c>
-      <c r="S27">
-        <v>0.28501261715933668</v>
-      </c>
-      <c r="T27">
-        <v>0.26438904508384675</v>
-      </c>
-      <c r="U27">
-        <v>0.22349486702672805</v>
-      </c>
-      <c r="V27">
-        <v>0.3000880766808377</v>
-      </c>
-      <c r="W27">
-        <v>0.28428339961702753</v>
-      </c>
-      <c r="X27">
-        <v>0.28949771689497716</v>
-      </c>
-      <c r="Y27">
-        <v>0.27546554222833963</v>
-      </c>
-      <c r="Z27">
-        <v>0.1712630286539932</v>
-      </c>
-      <c r="AA27">
-        <v>0.22976393784140595</v>
+        <v>0.19792026167823587</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>8.2835036602159899</v>
-      </c>
-      <c r="E28">
-        <v>6.8518331990330372</v>
-      </c>
-      <c r="F28">
-        <v>7.9203599247918337</v>
-      </c>
-      <c r="G28">
-        <v>6.9920091324200904</v>
-      </c>
-      <c r="H28">
-        <v>5.4123019070641956</v>
-      </c>
-      <c r="I28">
-        <v>4.2221588026382548</v>
-      </c>
-      <c r="J28">
-        <v>4.1714231354642308</v>
-      </c>
-      <c r="K28">
-        <v>3.3001966007102994</v>
-      </c>
-      <c r="L28">
-        <v>2.9783422120750886</v>
-      </c>
-      <c r="M28">
-        <v>2.378234398782344</v>
-      </c>
-      <c r="N28">
-        <v>2.1499238964992391</v>
-      </c>
-      <c r="O28">
-        <v>2.0682711821410451</v>
-      </c>
-      <c r="P28">
-        <v>1.9620433789954339</v>
-      </c>
-      <c r="Q28">
-        <v>1.5862823439878235</v>
-      </c>
-      <c r="R28">
-        <v>1.4856037544393708</v>
-      </c>
-      <c r="S28">
-        <v>1.3262620497209539</v>
-      </c>
-      <c r="T28">
-        <v>1.2810755961440894</v>
-      </c>
-      <c r="U28">
-        <v>1.2057648401826484</v>
-      </c>
-      <c r="V28">
-        <v>1.1589928970065957</v>
-      </c>
-      <c r="W28">
-        <v>1.0797184170471841</v>
-      </c>
-      <c r="X28">
-        <v>1.0170915778792491</v>
-      </c>
-      <c r="Y28">
-        <v>0.88232496194824972</v>
-      </c>
-      <c r="Z28">
-        <v>1.2390601217656012</v>
-      </c>
-      <c r="AA28">
-        <v>1.2319254185692541</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D29">
-        <v>0.11415525114155252</v>
+        <v>2000</v>
       </c>
       <c r="E29">
-        <v>0.11415525114155252</v>
+        <v>2001</v>
       </c>
       <c r="F29">
-        <v>0.11415525114155252</v>
+        <v>2002</v>
       </c>
       <c r="G29">
-        <v>7.6103500761035017E-2</v>
+        <v>2003</v>
       </c>
       <c r="H29">
-        <v>0.11415525114155252</v>
+        <v>2004</v>
       </c>
       <c r="I29">
-        <v>0.11415525114155252</v>
+        <v>2005</v>
       </c>
       <c r="J29">
-        <v>9.1324200913242004E-2</v>
+        <v>2006</v>
       </c>
       <c r="K29">
-        <v>4.1511000415110001E-2</v>
+        <v>2007</v>
       </c>
       <c r="L29">
-        <v>4.5186453576864537E-2</v>
+        <v>2008</v>
       </c>
       <c r="M29">
-        <v>6.1607595854171207E-2</v>
+        <v>2009</v>
       </c>
       <c r="N29">
-        <v>6.0565702688990357E-2</v>
+        <v>2010</v>
       </c>
       <c r="O29">
-        <v>9.3826233814974666E-2</v>
+        <v>2011</v>
       </c>
       <c r="P29">
-        <v>0.12822918621379872</v>
+        <v>2012</v>
       </c>
       <c r="Q29">
-        <v>0.13549268126146885</v>
+        <v>2013</v>
       </c>
       <c r="R29">
-        <v>0.13692492757892669</v>
+        <v>2014</v>
       </c>
       <c r="S29">
-        <v>0.13848341941762107</v>
+        <v>2015</v>
       </c>
       <c r="T29">
-        <v>0.13078439866398708</v>
+        <v>2016</v>
       </c>
       <c r="U29">
-        <v>0.14134611593860083</v>
+        <v>2017</v>
       </c>
       <c r="V29">
-        <v>0.12857366675067947</v>
+        <v>2018</v>
       </c>
       <c r="W29">
-        <v>0.12958015809982651</v>
+        <v>2019</v>
       </c>
       <c r="X29">
-        <v>0.1314419189044469</v>
+        <v>2020</v>
       </c>
       <c r="Y29">
-        <v>0.12647997737099445</v>
+        <v>2021</v>
       </c>
       <c r="Z29">
-        <v>0.1307021849389437</v>
+        <v>2022</v>
       </c>
       <c r="AA29">
-        <v>0.11879041402347462</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.45">
@@ -2494,78 +2314,576 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0.61522608801066792</v>
+      </c>
+      <c r="E30">
+        <v>0.62934286281516771</v>
+      </c>
+      <c r="F30">
+        <v>0.61410525614105249</v>
+      </c>
+      <c r="G30">
+        <v>0.63330715760695699</v>
+      </c>
+      <c r="H30">
+        <v>0.72548666186012989</v>
+      </c>
+      <c r="I30">
+        <v>0.74052659669098031</v>
+      </c>
+      <c r="J30">
+        <v>0.77363813512491642</v>
+      </c>
+      <c r="K30">
+        <v>0.75846709807546864</v>
+      </c>
+      <c r="L30">
+        <v>0.71674526536417393</v>
+      </c>
+      <c r="M30">
+        <v>0.66333456744415642</v>
+      </c>
+      <c r="N30">
+        <v>0.66085188356164382</v>
+      </c>
+      <c r="O30">
+        <v>0.62919014676012885</v>
+      </c>
+      <c r="P30">
+        <v>0.52921203606135103</v>
+      </c>
+      <c r="Q30">
+        <v>0.63624764974482939</v>
+      </c>
+      <c r="R30">
+        <v>0.68106183731909309</v>
+      </c>
+      <c r="S30">
+        <v>0.70676749919842574</v>
+      </c>
+      <c r="T30">
+        <v>0.69930259547283602</v>
+      </c>
+      <c r="U30">
+        <v>0.69169425869419376</v>
+      </c>
+      <c r="V30">
+        <v>0.67662443458314581</v>
+      </c>
+      <c r="W30">
+        <v>0.69304680906316962</v>
+      </c>
+      <c r="X30">
+        <v>0.69550645885530227</v>
+      </c>
+      <c r="Y30">
+        <v>0.68029990954762931</v>
+      </c>
+      <c r="Z30">
+        <v>0.64195219167132056</v>
+      </c>
+      <c r="AA30">
+        <v>0.60575494311218137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.34602076124567482</v>
+      </c>
+      <c r="E31">
+        <v>0.42117978124668154</v>
+      </c>
+      <c r="F31">
+        <v>0.47055856429860893</v>
+      </c>
+      <c r="G31">
+        <v>0.51515875544228529</v>
+      </c>
+      <c r="H31">
+        <v>0.62231700981598448</v>
+      </c>
+      <c r="I31">
+        <v>0.57221959796357535</v>
+      </c>
+      <c r="J31">
+        <v>0.58009237390437207</v>
+      </c>
+      <c r="K31">
+        <v>0.57878024458090593</v>
+      </c>
+      <c r="L31">
+        <v>0.61000827129859381</v>
+      </c>
+      <c r="M31">
+        <v>0.52024422939968995</v>
+      </c>
+      <c r="N31">
+        <v>0.45490352335545442</v>
+      </c>
+      <c r="O31">
+        <v>0.51215289704730615</v>
+      </c>
+      <c r="P31">
+        <v>0.56264684464351955</v>
+      </c>
+      <c r="Q31">
+        <v>0.51638935070050329</v>
+      </c>
+      <c r="R31">
+        <v>0.50458246816891728</v>
+      </c>
+      <c r="S31">
+        <v>0.50892743542983165</v>
+      </c>
+      <c r="T31">
+        <v>0.46671280059135295</v>
+      </c>
+      <c r="U31">
+        <v>0.43565916312852143</v>
+      </c>
+      <c r="V31">
+        <v>0.38011695906432741</v>
+      </c>
+      <c r="W31">
+        <v>0.25154209725226306</v>
+      </c>
+      <c r="X31">
+        <v>0.19733814732221869</v>
+      </c>
+      <c r="Y31">
+        <v>0.23501565653517861</v>
+      </c>
+      <c r="Z31">
+        <v>0.37900884409845853</v>
+      </c>
+      <c r="AA31">
+        <v>0.25717309414385414</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>0.21688427845750258</v>
+      </c>
+      <c r="E32">
+        <v>0.22202418548512892</v>
+      </c>
+      <c r="F32">
+        <v>0.21195692035826924</v>
+      </c>
+      <c r="G32">
+        <v>0.2444397765407833</v>
+      </c>
+      <c r="H32">
+        <v>0.25723564401629956</v>
+      </c>
+      <c r="I32">
+        <v>0.28042118198664318</v>
+      </c>
+      <c r="J32">
+        <v>0.28071079794005777</v>
+      </c>
+      <c r="K32">
+        <v>0.2922584260992816</v>
+      </c>
+      <c r="L32">
+        <v>0.2779788969658355</v>
+      </c>
+      <c r="M32">
+        <v>0.23646215642703375</v>
+      </c>
+      <c r="N32">
+        <v>0.24074060070301742</v>
+      </c>
+      <c r="O32">
+        <v>0.22510363173419468</v>
+      </c>
+      <c r="P32">
+        <v>0.20133855684813015</v>
+      </c>
+      <c r="Q32">
+        <v>0.17523112617091591</v>
+      </c>
+      <c r="R32">
+        <v>0.15844369919854487</v>
+      </c>
+      <c r="S32">
+        <v>0.20478133387114289</v>
+      </c>
+      <c r="T32">
+        <v>0.24738866431689593</v>
+      </c>
+      <c r="U32">
+        <v>0.2791433980876013</v>
+      </c>
+      <c r="V32">
+        <v>0.25589885068453339</v>
+      </c>
+      <c r="W32">
+        <v>0.28175925948019492</v>
+      </c>
+      <c r="X32">
+        <v>0.27138259384113744</v>
+      </c>
+      <c r="Y32">
+        <v>0.2955149688458561</v>
+      </c>
+      <c r="Z32">
+        <v>0.2867461537463678</v>
+      </c>
+      <c r="AA32">
+        <v>0.23584379225019769</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>0.30785003663554733</v>
+      </c>
+      <c r="E33">
+        <v>0.3246419991455694</v>
+      </c>
+      <c r="F33">
+        <v>0.27242847373877754</v>
+      </c>
+      <c r="G33">
+        <v>0.25066305744675033</v>
+      </c>
+      <c r="H33">
+        <v>0.2878697637482629</v>
+      </c>
+      <c r="I33">
+        <v>0.24164201341994127</v>
+      </c>
+      <c r="J33">
+        <v>0.24679151021192447</v>
+      </c>
+      <c r="K33">
+        <v>0.21833189641408821</v>
+      </c>
+      <c r="L33">
+        <v>0.27431533213114406</v>
+      </c>
+      <c r="M33">
+        <v>0.32220499948856351</v>
+      </c>
+      <c r="N33">
+        <v>0.33232439853964491</v>
+      </c>
+      <c r="O33">
+        <v>0.29418411739628436</v>
+      </c>
+      <c r="P33">
+        <v>0.26672323467058051</v>
+      </c>
+      <c r="Q33">
+        <v>0.33373809433461088</v>
+      </c>
+      <c r="R33">
+        <v>0.36886258026147345</v>
+      </c>
+      <c r="S33">
+        <v>0.28501261715933668</v>
+      </c>
+      <c r="T33">
+        <v>0.26438904508384675</v>
+      </c>
+      <c r="U33">
+        <v>0.22349486702672805</v>
+      </c>
+      <c r="V33">
+        <v>0.3000880766808377</v>
+      </c>
+      <c r="W33">
+        <v>0.28428339961702753</v>
+      </c>
+      <c r="X33">
+        <v>0.28949771689497716</v>
+      </c>
+      <c r="Y33">
+        <v>0.27546554222833963</v>
+      </c>
+      <c r="Z33">
+        <v>0.1712630286539932</v>
+      </c>
+      <c r="AA33">
+        <v>0.22976393784140595</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>8.2835036602159899</v>
+      </c>
+      <c r="E34">
+        <v>6.8518331990330372</v>
+      </c>
+      <c r="F34">
+        <v>7.9203599247918337</v>
+      </c>
+      <c r="G34">
+        <v>6.9920091324200904</v>
+      </c>
+      <c r="H34">
+        <v>5.4123019070641956</v>
+      </c>
+      <c r="I34">
+        <v>4.2221588026382548</v>
+      </c>
+      <c r="J34">
+        <v>4.1714231354642308</v>
+      </c>
+      <c r="K34">
+        <v>3.3001966007102994</v>
+      </c>
+      <c r="L34">
+        <v>2.9783422120750886</v>
+      </c>
+      <c r="M34">
+        <v>2.378234398782344</v>
+      </c>
+      <c r="N34">
+        <v>2.1499238964992391</v>
+      </c>
+      <c r="O34">
+        <v>2.0682711821410451</v>
+      </c>
+      <c r="P34">
+        <v>1.9620433789954339</v>
+      </c>
+      <c r="Q34">
+        <v>1.5862823439878235</v>
+      </c>
+      <c r="R34">
+        <v>1.4856037544393708</v>
+      </c>
+      <c r="S34">
+        <v>1.3262620497209539</v>
+      </c>
+      <c r="T34">
+        <v>1.2810755961440894</v>
+      </c>
+      <c r="U34">
+        <v>1.2057648401826484</v>
+      </c>
+      <c r="V34">
+        <v>1.1589928970065957</v>
+      </c>
+      <c r="W34">
+        <v>1.0797184170471841</v>
+      </c>
+      <c r="X34">
+        <v>1.0170915778792491</v>
+      </c>
+      <c r="Y34">
+        <v>0.88232496194824972</v>
+      </c>
+      <c r="Z34">
+        <v>1.2390601217656012</v>
+      </c>
+      <c r="AA34">
+        <v>1.2319254185692541</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="E35">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="F35">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="G35">
+        <v>7.6103500761035017E-2</v>
+      </c>
+      <c r="H35">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="I35">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="J35">
+        <v>9.1324200913242004E-2</v>
+      </c>
+      <c r="K35">
+        <v>4.1511000415110001E-2</v>
+      </c>
+      <c r="L35">
+        <v>4.5186453576864537E-2</v>
+      </c>
+      <c r="M35">
+        <v>6.1607595854171207E-2</v>
+      </c>
+      <c r="N35">
+        <v>6.0565702688990357E-2</v>
+      </c>
+      <c r="O35">
+        <v>9.3826233814974666E-2</v>
+      </c>
+      <c r="P35">
+        <v>0.12822918621379872</v>
+      </c>
+      <c r="Q35">
+        <v>0.13549268126146885</v>
+      </c>
+      <c r="R35">
+        <v>0.13692492757892669</v>
+      </c>
+      <c r="S35">
+        <v>0.13848341941762107</v>
+      </c>
+      <c r="T35">
+        <v>0.13078439866398708</v>
+      </c>
+      <c r="U35">
+        <v>0.14134611593860083</v>
+      </c>
+      <c r="V35">
+        <v>0.12857366675067947</v>
+      </c>
+      <c r="W35">
+        <v>0.12958015809982651</v>
+      </c>
+      <c r="X35">
+        <v>0.1314419189044469</v>
+      </c>
+      <c r="Y35">
+        <v>0.12647997737099445</v>
+      </c>
+      <c r="Z35">
+        <v>0.1307021849389437</v>
+      </c>
+      <c r="AA35">
+        <v>0.11879041402347462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="D30">
+      <c r="D36">
         <v>0.1775748351090817</v>
       </c>
-      <c r="E30">
+      <c r="E36">
         <v>0.20409575204095751</v>
       </c>
-      <c r="F30">
+      <c r="F36">
         <v>0.20489404051047885</v>
       </c>
-      <c r="G30">
+      <c r="G36">
         <v>0.19157088122605365</v>
       </c>
-      <c r="H30">
+      <c r="H36">
         <v>0.18588111690305897</v>
       </c>
-      <c r="I30">
+      <c r="I36">
         <v>0.16387931758971341</v>
       </c>
-      <c r="J30">
+      <c r="J36">
         <v>0.17844268204758473</v>
       </c>
-      <c r="K30">
+      <c r="K36">
         <v>0.17038728225942837</v>
       </c>
-      <c r="L30">
+      <c r="L36">
         <v>0.15716558655749158</v>
       </c>
-      <c r="M30">
+      <c r="M36">
         <v>0.15298675050527735</v>
       </c>
-      <c r="N30">
+      <c r="N36">
         <v>0.17980930749757493</v>
       </c>
-      <c r="O30">
+      <c r="O36">
         <v>0.16248977221738325</v>
       </c>
-      <c r="P30">
+      <c r="P36">
         <v>0.18899036022323698</v>
       </c>
-      <c r="Q30">
+      <c r="Q36">
         <v>0.19917016885352842</v>
       </c>
-      <c r="R30">
+      <c r="R36">
         <v>0.19964017423142477</v>
       </c>
-      <c r="S30">
+      <c r="S36">
         <v>0.18534616268497148</v>
       </c>
-      <c r="T30">
+      <c r="T36">
         <v>0.21528852800576376</v>
       </c>
-      <c r="U30">
+      <c r="U36">
         <v>0.20791726439950117</v>
       </c>
-      <c r="V30">
+      <c r="V36">
         <v>0.19773519552573904</v>
       </c>
-      <c r="W30">
+      <c r="W36">
         <v>0.21591161732765551</v>
       </c>
-      <c r="X30">
+      <c r="X36">
         <v>0.19701495045221024</v>
       </c>
-      <c r="Y30">
+      <c r="Y36">
         <v>0.21237950279046169</v>
       </c>
-      <c r="Z30">
+      <c r="Z36">
         <v>0.19586027860834898</v>
       </c>
-      <c r="AA30">
+      <c r="AA36">
         <v>0.21801705559203086</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-29 00:50
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB53522-D689-4D07-BDAB-15E568CCE188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344268BD-C277-4A12-94C0-0274EF9FCE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -338,10 +338,10 @@
     <t>ISO</t>
   </si>
   <si>
+    <t>Import</t>
+  </si>
+  <si>
     <t>Export</t>
-  </si>
-  <si>
-    <t>Import</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1639,76 @@
         <v>85</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>44.35</v>
+      </c>
+      <c r="D14">
+        <v>48.38</v>
+      </c>
+      <c r="E14">
+        <v>50.6</v>
+      </c>
+      <c r="F14">
+        <v>50.97</v>
+      </c>
+      <c r="G14">
+        <v>45.63</v>
+      </c>
+      <c r="H14">
+        <v>49.15</v>
+      </c>
+      <c r="I14">
+        <v>44.99</v>
+      </c>
+      <c r="J14">
+        <v>46.28</v>
+      </c>
+      <c r="K14">
+        <v>40.03</v>
+      </c>
+      <c r="L14">
+        <v>44.96</v>
+      </c>
+      <c r="M14">
+        <v>44.16</v>
+      </c>
+      <c r="N14">
+        <v>45.73</v>
+      </c>
+      <c r="O14">
+        <v>43.1</v>
+      </c>
+      <c r="P14">
+        <v>42.14</v>
+      </c>
+      <c r="Q14">
+        <v>43.72</v>
+      </c>
+      <c r="R14">
+        <v>46.38</v>
+      </c>
+      <c r="S14">
+        <v>37.03</v>
+      </c>
+      <c r="T14">
+        <v>37.76</v>
+      </c>
+      <c r="U14">
+        <v>43.9</v>
+      </c>
+      <c r="V14">
+        <v>38.14</v>
+      </c>
+      <c r="W14">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="X14">
+        <v>42.79</v>
+      </c>
+      <c r="Y14">
+        <v>42.99</v>
+      </c>
+      <c r="Z14">
+        <v>51.25</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.45">
@@ -1650,7 +1719,76 @@
         <v>86</v>
       </c>
       <c r="C15">
-        <v>44.35</v>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-29 01:00
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344268BD-C277-4A12-94C0-0274EF9FCE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217B9FC9-91A7-4E09-863D-4425C7C3956D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,7 +332,7 @@
     <t>Unnamed: 25</t>
   </si>
   <si>
-    <t>Electricity Trade Data (TWh)</t>
+    <t>Electricity Trade Data (TWh) - Source: EMBER (estimated)</t>
   </si>
   <si>
     <t>ISO</t>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 10:07
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3824E455-BCD0-42DE-8AB3-D2566157C90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926BABD6-BFAE-467C-918F-A275AC7B67DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="72">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -211,6 +211,24 @@
   </si>
   <si>
     <t>CCGT - CHP</t>
+  </si>
+  <si>
+    <t>~UC_T: FX</t>
+  </si>
+  <si>
+    <t>pset_pn</t>
+  </si>
+  <si>
+    <t>UCE_Solar capacity aggregation for peak</t>
+  </si>
+  <si>
+    <t>ElcAgg_Solar</t>
+  </si>
+  <si>
+    <t>UCE_Wind capacity aggregation for peak</t>
+  </si>
+  <si>
+    <t>ElcAgg_Wind</t>
   </si>
   <si>
     <t>EMBER Utilization Factors</t>
@@ -717,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AJ27"/>
+  <dimension ref="B1:AJ40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -765,19 +783,19 @@
     </row>
     <row r="2" spans="2:36" x14ac:dyDescent="0.45">
       <c r="F2" s="10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.45">
@@ -785,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4">
         <v>0.52921203606135103</v>
@@ -860,7 +878,7 @@
         <v>0.14275360852558924</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1273,6 +1291,72 @@
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L27" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="E35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1306,12 +1390,12 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B2" s="7">
         <v>2000</v>
@@ -1388,7 +1472,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
         <v>0.61522608801066792</v>
@@ -1927,12 +2011,12 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B16" s="7">
         <v>2000</v>
@@ -2006,7 +2090,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B17" s="4">
         <v>0.29387335196920444</v>
@@ -2080,7 +2164,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B18" s="4">
         <v>0.91033975698475367</v>
@@ -2450,12 +2534,12 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B31" s="7">
         <v>2000</v>
@@ -2532,7 +2616,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B32" s="8">
         <v>269.94</v>
@@ -2609,7 +2693,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B33" s="9">
         <v>6.09</v>
@@ -3225,12 +3309,12 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B45" s="7">
         <v>2000</v>
@@ -3304,7 +3388,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B46" s="8">
         <v>276.64163499999995</v>
@@ -3378,7 +3462,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B47" s="9">
         <v>1.3939999999999999</v>
@@ -3600,7 +3684,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B50" s="9">
         <v>4.7050000000000001</v>
@@ -3970,12 +4054,12 @@
     </row>
     <row r="58" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B59" s="7">
         <v>2000</v>
@@ -4052,7 +4136,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B60" s="9">
         <v>1.1299999999999999</v>
@@ -4668,12 +4752,12 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A70" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B71" s="7">
         <v>2000</v>
@@ -4753,7 +4837,7 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B72" s="9">
         <v>0.54149999999999998</v>
@@ -4833,7 +4917,7 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B73" s="9">
         <v>0.59</v>
@@ -5234,12 +5318,12 @@
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="85" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="7" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>27</v>
@@ -5319,10 +5403,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B87" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C87" s="9">
         <v>44.35</v>
@@ -5399,10 +5483,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B88" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C88" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 18:24
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B46235-61FB-4409-B9E8-D8F1703CF08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CA36CE-5727-44BF-BC8B-E6BBE992B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="74">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>ep*,EN*</t>
+  </si>
+  <si>
+    <t>Geothermal*</t>
   </si>
   <si>
     <t>EMBER Utilization Factors</t>
@@ -741,7 +744,7 @@
   <dimension ref="B1:AJ40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -786,19 +789,19 @@
     </row>
     <row r="2" spans="2:36" x14ac:dyDescent="0.45">
       <c r="F2" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.45">
@@ -806,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3" s="4">
         <v>0.52921203606135103</v>
@@ -881,7 +884,7 @@
         <v>0.14275360852558924</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1166,8 +1169,8 @@
         <v>2100</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,L15:L27)</f>
-        <v>Bioenergy + CCUS,Bioenergy - Cofiring,Bioenergy - Large scale unit,Bioenergy - Medium-scale CHP,Concentrating solar power,Fuel cell (distributed electricity generation),Marine,Oxyfuel + CCS,Solar photovoltaics - Buildings,Solar photovoltaics - Large scale unit,Wind offshore,Wind onshore,CCGT - CHP</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,L15:L28)</f>
+        <v>Bioenergy + CCUS,Bioenergy - Cofiring,Bioenergy - Large scale unit,Bioenergy - Medium-scale CHP,Concentrating solar power,Fuel cell (distributed electricity generation),Marine,Oxyfuel + CCS,Solar photovoltaics - Buildings,Solar photovoltaics - Large scale unit,Wind offshore,Wind onshore,CCGT - CHP,Geothermal*</v>
       </c>
       <c r="L15" t="s">
         <v>30</v>
@@ -1294,6 +1297,11 @@
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L27" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.45">
@@ -1393,12 +1401,12 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7">
         <v>2000</v>
@@ -1475,7 +1483,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4">
         <v>0.61522608801066792</v>
@@ -2014,12 +2022,12 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" s="7">
         <v>2000</v>
@@ -2093,7 +2101,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4">
         <v>0.29387335196920444</v>
@@ -2167,7 +2175,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="4">
         <v>0.91033975698475367</v>
@@ -2537,12 +2545,12 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" s="7">
         <v>2000</v>
@@ -2619,7 +2627,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B32" s="8">
         <v>269.94</v>
@@ -2696,7 +2704,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B33" s="9">
         <v>6.09</v>
@@ -3312,12 +3320,12 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B45" s="7">
         <v>2000</v>
@@ -3391,7 +3399,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B46" s="8">
         <v>276.64163499999995</v>
@@ -3465,7 +3473,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" s="9">
         <v>1.3939999999999999</v>
@@ -3687,7 +3695,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B50" s="9">
         <v>4.7050000000000001</v>
@@ -4057,12 +4065,12 @@
     </row>
     <row r="58" spans="1:25" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B59" s="7">
         <v>2000</v>
@@ -4139,7 +4147,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B60" s="9">
         <v>1.1299999999999999</v>
@@ -4755,12 +4763,12 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A70" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B71" s="7">
         <v>2000</v>
@@ -4840,7 +4848,7 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B72" s="9">
         <v>0.54149999999999998</v>
@@ -4920,7 +4928,7 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B73" s="9">
         <v>0.59</v>
@@ -5321,12 +5329,12 @@
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="85" spans="1:26" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>27</v>
@@ -5406,10 +5414,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C87" s="9">
         <v>44.35</v>
@@ -5486,10 +5494,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B88" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C88" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-06 12:25
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2DF5CA3-64B2-4505-947F-6EDD71040366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196D1765-7267-4B35-A0CB-4F67ACC1D76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,11 +306,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,19 +339,12 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,18 +353,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4F81BD"/>
+        <fgColor rgb="FFDCE6F1"/>
         <bgColor rgb="FFDCE6F1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7F9FC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -380,58 +366,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,11 +729,10 @@
     <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.59765625" customWidth="1"/>
     <col min="5" max="5" width="9.53125" customWidth="1"/>
-    <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.9296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.06640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.19921875" bestFit="1" customWidth="1"/>
@@ -806,7 +755,7 @@
     <col min="36" max="36" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="AA1">
         <v>1.1000000000000001</v>
       </c>
@@ -814,47 +763,47 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="F2" s="6" t="s">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="F2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="4">
         <v>0.52921203606135103</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="4">
         <v>0.77363813512491642</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="4">
         <v>0.29387335196920444</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="4">
         <v>0.65763867133730136</v>
       </c>
       <c r="V3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -867,43 +816,43 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="4">
         <v>0.19733814732221869</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="4">
         <v>0.62231700981598448</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <f>IFERROR(VLOOKUP(B5,$F$3:$J$11,5,FALSE),"")</f>
         <v>0.31127604163438005</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="4">
         <v>0.15844369919854487</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="4">
         <v>0.2955149688458561</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A6" s="5">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
         <v>0.28000000000000003</v>
       </c>
       <c r="B6" t="s">
@@ -912,19 +861,19 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <f>IFERROR(MIN(VLOOKUP(B6,$F$3:$J$11,5,FALSE),$A$6),"")</f>
         <v>0.14275360852558924</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="13">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
         <v>0.79908675799086759</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="4">
         <v>0.96681069431997602</v>
       </c>
       <c r="U6" t="s">
@@ -934,30 +883,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <f t="shared" ref="D7" si="0">IFERROR(VLOOKUP(B7,$F$3:$J$11,5,FALSE),"")</f>
         <v>0.21594436217582091</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="4">
         <v>0.1712630286539932</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="4">
         <v>0.36886258026147345</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="4">
         <v>0.15125668935897063</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="4">
         <v>0.31127604163438005</v>
       </c>
       <c r="U7" t="s">
@@ -1006,24 +955,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <f>IFERROR(VLOOKUP(B8,$F$3:$J$11,3,FALSE),"")</f>
         <v>0</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="U8" t="s">
         <v>20</v>
       </c>
@@ -1076,20 +1025,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="F9" s="7" t="s">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="4">
         <v>0.88232496194824972</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="4">
         <v>8.2835036602159899</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="4">
         <v>2.1681649145671975E-2</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="4">
         <v>0.18947752518915301</v>
       </c>
       <c r="U9" t="s">
@@ -1144,37 +1093,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="F10" s="9" t="s">
+    <row r="10" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="4">
         <v>4.1511000415110001E-2</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="4">
         <v>0.14134611593860083</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="4">
         <v>4.0424449979244499E-2</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="4">
         <v>0.14275360852558924</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="F11" s="7" t="s">
+    <row r="11" spans="1:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="4">
         <v>0.15298675050527735</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="4">
         <v>0.21801705559203086</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="4">
         <v>0.15299618343829349</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="4">
         <v>0.21594436217582091</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-21 23:20
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F902FFA0-E1CE-4E6E-8119-38C1420E578C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4C1D68A-C3FB-49E6-9AF6-E1E632EFFC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,7 +618,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{140B6347-BEB8-56A1-41AF-C48A0E245F24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39B1709F-8471-6028-164B-82A49FCA43AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>